<commit_message>
obtained ADD for all faulkner novels and added to master spreadsheet
</commit_message>
<xml_diff>
--- a/src/results/Faulkner-Master-Spreadsheet.xlsx
+++ b/src/results/Faulkner-Master-Spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan McFalls\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Stanford University\2017-2018 Year\Spring 2018\Senior Capstone Project\Project\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Title</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>#79997</t>
+  </si>
+  <si>
+    <t>Average dependency distance</t>
   </si>
 </sst>
 </file>
@@ -1063,11 +1066,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="338984992"/>
-        <c:axId val="339047456"/>
+        <c:axId val="337367176"/>
+        <c:axId val="337546256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="338984992"/>
+        <c:axId val="337367176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1124,7 +1127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339047456"/>
+        <c:crossAx val="337546256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1132,7 +1135,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="339047456"/>
+        <c:axId val="337546256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8"/>
@@ -1185,7 +1188,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338984992"/>
+        <c:crossAx val="337367176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1482,11 +1485,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="339047848"/>
-        <c:axId val="339045888"/>
+        <c:axId val="337547432"/>
+        <c:axId val="337546648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="339047848"/>
+        <c:axId val="337547432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1543,7 +1546,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339045888"/>
+        <c:crossAx val="337546648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1551,7 +1554,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="339045888"/>
+        <c:axId val="337546648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1602,7 +1605,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339047848"/>
+        <c:crossAx val="337547432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1897,11 +1900,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="340937056"/>
-        <c:axId val="340938232"/>
+        <c:axId val="337547040"/>
+        <c:axId val="337548216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="340937056"/>
+        <c:axId val="337547040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,7 +1961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340938232"/>
+        <c:crossAx val="337548216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1966,7 +1969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="340938232"/>
+        <c:axId val="337548216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2017,7 +2020,342 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340937056"/>
+        <c:crossAx val="337547040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average dependency distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$O$2:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>3.1388615280000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2187536950000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2341488090000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0680102790000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1933339890000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.163553759</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1591647520000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1862311060000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2267937899999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.390706512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1341369270000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3358912630000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.2073623709999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1873630930000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.3819969419999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.1841314700000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.1879830600000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.3380344430000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.4347044599999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="371776520"/>
+        <c:axId val="372797520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="371776520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="372797520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="372797520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="371776520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2186,6 +2524,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3193,6 +3571,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3782,6 +4663,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4053,11 +4964,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N80"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4074,10 +4985,11 @@
     <col min="11" max="11" width="15.21875" customWidth="1"/>
     <col min="12" max="12" width="11.44140625" customWidth="1"/>
     <col min="13" max="13" width="14.5546875" customWidth="1"/>
-    <col min="14" max="14" width="23.88671875" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4120,8 +5032,11 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4164,8 +5079,11 @@
       <c r="N2">
         <v>3.20820652744254</v>
       </c>
+      <c r="O2">
+        <v>3.1388615280000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4208,8 +5126,11 @@
       <c r="N3">
         <v>3.36902619476104</v>
       </c>
+      <c r="O3">
+        <v>3.2187536950000002</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4252,8 +5173,11 @@
       <c r="N4">
         <v>4.4730434782608697</v>
       </c>
+      <c r="O4">
+        <v>3.2341488090000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4296,8 +5220,11 @@
       <c r="N5">
         <v>3.3144413069786198</v>
       </c>
+      <c r="O5">
+        <v>3.0680102790000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -4340,8 +5267,11 @@
       <c r="N6">
         <v>3.6854599406528101</v>
       </c>
+      <c r="O6">
+        <v>3.1933339890000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -4384,8 +5314,11 @@
       <c r="N7">
         <v>3.63794637183886</v>
       </c>
+      <c r="O7">
+        <v>3.163553759</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -4428,8 +5361,11 @@
       <c r="N8">
         <v>4.1919431279620802</v>
       </c>
+      <c r="O8">
+        <v>3.1591647520000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -4472,8 +5408,11 @@
       <c r="N9">
         <v>4.3444922386384803</v>
       </c>
+      <c r="O9">
+        <v>3.1862311060000001</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -4516,8 +5455,11 @@
       <c r="N10">
         <v>7.1794516754361597</v>
       </c>
+      <c r="O10">
+        <v>3.2267937899999999</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -4560,8 +5502,11 @@
       <c r="N11">
         <v>4.6283141570785302</v>
       </c>
+      <c r="O11">
+        <v>3.390706512</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -4604,8 +5549,11 @@
       <c r="N12">
         <v>4.46451725950587</v>
       </c>
+      <c r="O12">
+        <v>3.1341369270000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -4648,8 +5596,11 @@
       <c r="N13">
         <v>5.0429942418426101</v>
       </c>
+      <c r="O13">
+        <v>3.3358912630000002</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -4692,8 +5643,11 @@
       <c r="N14">
         <v>4.6103662524525797</v>
       </c>
+      <c r="O14">
+        <v>3.2073623709999999</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -4736,8 +5690,11 @@
       <c r="N15">
         <v>5.9487964989059003</v>
       </c>
+      <c r="O15">
+        <v>3.1873630930000001</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -4780,8 +5737,11 @@
       <c r="N16">
         <v>4.5312117503059897</v>
       </c>
+      <c r="O16">
+        <v>3.3819969419999998</v>
+      </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -4824,8 +5784,11 @@
       <c r="N17">
         <v>5.2939612015018698</v>
       </c>
+      <c r="O17">
+        <v>3.1841314700000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -4868,8 +5831,11 @@
       <c r="N18">
         <v>4.7897132453345401</v>
       </c>
+      <c r="O18">
+        <v>3.1879830600000001</v>
+      </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -4912,8 +5878,11 @@
       <c r="N19">
         <v>5.1421009771986901</v>
       </c>
+      <c r="O19">
+        <v>3.3380344430000002</v>
+      </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -4956,13 +5925,16 @@
       <c r="N20">
         <v>4.1295433364398804</v>
       </c>
+      <c r="O20">
+        <v>3.4347044599999998</v>
+      </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -5019,7 +5991,7 @@
         <v>3.6146873033224565</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -5076,7 +6048,7 @@
         <v>4.9231541361309024</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -5133,7 +6105,7 @@
         <v>4.9725545016144785</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -5190,7 +6162,7 @@
         <v>4.6646661686205801</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -5247,7 +6219,7 @@
         <v>4.1360406843699602</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -5304,7 +6276,7 @@
         <v>4.6894031505624829</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
added a few charts to the master spreadsheet
</commit_message>
<xml_diff>
--- a/src/results/Faulkner-Master-Spreadsheet.xlsx
+++ b/src/results/Faulkner-Master-Spreadsheet.xlsx
@@ -1066,11 +1066,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="337367176"/>
-        <c:axId val="337546256"/>
+        <c:axId val="340109600"/>
+        <c:axId val="341691976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="337367176"/>
+        <c:axId val="340109600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1127,7 +1127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337546256"/>
+        <c:crossAx val="341691976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1135,7 +1135,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="337546256"/>
+        <c:axId val="341691976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8"/>
@@ -1188,7 +1188,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337367176"/>
+        <c:crossAx val="340109600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1485,11 +1485,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="337547432"/>
-        <c:axId val="337546648"/>
+        <c:axId val="341690408"/>
+        <c:axId val="341691192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="337547432"/>
+        <c:axId val="341690408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1546,7 +1546,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337546648"/>
+        <c:crossAx val="341691192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1554,7 +1554,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="337546648"/>
+        <c:axId val="341691192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1605,7 +1605,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337547432"/>
+        <c:crossAx val="341690408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1900,11 +1900,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="337547040"/>
-        <c:axId val="337548216"/>
+        <c:axId val="341692368"/>
+        <c:axId val="341689624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="337547040"/>
+        <c:axId val="341692368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1961,7 +1961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337548216"/>
+        <c:crossAx val="341689624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1969,7 +1969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="337548216"/>
+        <c:axId val="341689624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2020,7 +2020,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337547040"/>
+        <c:crossAx val="341692368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2172,6 +2172,71 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Faulkner-Basic-Metrics-Results'!$O$2:$O$20</c:f>
@@ -2250,16 +2315,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="371776520"/>
-        <c:axId val="372797520"/>
+        <c:axId val="341688840"/>
+        <c:axId val="341689232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="371776520"/>
+        <c:axId val="341688840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2296,7 +2362,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="372797520"/>
+        <c:crossAx val="341689232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2304,7 +2370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="372797520"/>
+        <c:axId val="341689232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2355,7 +2421,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371776520"/>
+        <c:crossAx val="341688840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2367,6 +2433,2181 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Part of Speech Percentages</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Noun%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$I$2:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.21539444338597</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22097471063897201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23764831707109099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.21580375090259701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.204102077401666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.229816716004282</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18374271934217101</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20812087096812101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.193609840246006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.200808742535799</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20515372017330999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.20574206959394001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.20716544294978201</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.20551782458180201</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.224367359040094</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.204344695902588</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.20558068670876101</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.199962937876212</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.20692364959880799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Verb%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$J$2:$J$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.23214946148587301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21365149833518299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.192519627066363</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.246082238832185</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24160778937748201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.21802607545506</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22829639195635501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21130044631816899</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.21204530113252801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22891182097512899</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20598295913924899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.21006321544507001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.20538792718437901</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.19244998810813599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.18856275833202499</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.190590665790215</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.21585304558162899</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.216193592086597</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2313570187774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adjective%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$K$2:$K$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>8.0861174308224995E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1358014904074794E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9213522331842701E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5904256357213906E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9263946008646998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4646973609623903E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1493556123659102E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3862359715957898E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5911647791194697E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9032407675807197E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.95316872939859E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.4995159177629699E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0403915894027905E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.8774609550487503E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.92828615776347E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.3215012364228199E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8341029749002594E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.23030914923255E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8192158160311003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adverb%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$L$2:$L$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>7.3038430071614993E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5937450451878802E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7867411707264097E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0968560332546199E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3183591690393304E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0741953769603799E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.7288827978810296E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.8405972891176096E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8457211430285704E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.23815873383964E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.4851877189709102E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.3988268124608398E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.7276917305321805E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.7830395602653206E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.8840056506043E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.2759883557141501E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.4186850124084995E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.5984510588265307E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.6668458929605405E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pronoun%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$M$2:$M$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.14048438252995099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.123434279372126</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10612178468739999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.124899982435939</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13074273260923</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.121660263273918</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12832406504493499</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.103512841951552</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10228005700142501</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.113948634703461</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.105593216825258</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.106256051027962</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.107454847526662</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.8173938320868903E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.2770888923769104E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.4612952702914199E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.10394873244746</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.10510307104425699</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.10573662006783</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="376164408"/>
+        <c:axId val="376161664"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="376164408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="376161664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="376161664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="376164408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Part of Speech Percentages</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Noun%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$I$2:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.21539444338597</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22097471063897201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23764831707109099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.21580375090259701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.204102077401666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.229816716004282</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18374271934217101</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20812087096812101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.193609840246006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.200808742535799</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20515372017330999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.20574206959394001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.20716544294978201</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.20551782458180201</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.224367359040094</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.204344695902588</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.20558068670876101</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.199962937876212</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.20692364959880799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Verb%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$J$2:$J$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.23214946148587301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21365149833518299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.192519627066363</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.246082238832185</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24160778937748201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.21802607545506</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22829639195635501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21130044631816899</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.21204530113252801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22891182097512899</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20598295913924899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.21006321544507001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.20538792718437901</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.19244998810813599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.18856275833202499</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.190590665790215</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.21585304558162899</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.216193592086597</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2313570187774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adjective%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$K$2:$K$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>8.0861174308224995E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1358014904074794E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9213522331842701E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5904256357213906E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9263946008646998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4646973609623903E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1493556123659102E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3862359715957898E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5911647791194697E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9032407675807197E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.95316872939859E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.4995159177629699E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0403915894027905E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.8774609550487503E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.92828615776347E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.3215012364228199E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8341029749002594E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.23030914923255E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8192158160311003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adverb%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$L$2:$L$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>7.3038430071614993E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5937450451878802E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7867411707264097E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0968560332546199E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3183591690393304E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0741953769603799E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.7288827978810296E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.8405972891176096E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8457211430285704E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.23815873383964E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.4851877189709102E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.3988268124608398E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.7276917305321805E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.7830395602653206E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.8840056506043E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.2759883557141501E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.4186850124084995E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.5984510588265307E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.6668458929605405E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pronoun%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Soldiers' Pay</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mosquitoes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flags in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Sound and the Fury</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>As I Lay Dying</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sanctuary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Light in August</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pylon</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Absalom! Absalom!</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>The Unvanquished</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>The Wild Palms</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>The Hamlet</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Go Down, Moses</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Intruder in the Dust</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Requiem for a Nun</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>A Fable</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Town</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Mansion</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>The Reivers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Faulkner-Basic-Metrics-Results'!$M$2:$M$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.14048438252995099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.123434279372126</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10612178468739999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.124899982435939</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13074273260923</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.121660263273918</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12832406504493499</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.103512841951552</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10228005700142501</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.113948634703461</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.105593216825258</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.106256051027962</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.107454847526662</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.8173938320868903E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.2770888923769104E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.4612952702914199E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.10394873244746</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.10510307104425699</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.10573662006783</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="379217672"/>
+        <c:axId val="379220808"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="379217672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379220808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="379220808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379217672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2564,6 +4805,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4576,20 +6897,1026 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>975360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4611,15 +7938,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:colOff>922020</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>998220</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4670,16 +7997,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4693,6 +8020,68 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>944880</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1531620</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4962,13 +8351,265 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4472C4"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1:O20"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>